<commit_message>
minor revision for TSMC
</commit_message>
<xml_diff>
--- a/SourceDetection/data/result.xlsx
+++ b/SourceDetection/data/result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="scale-free SI" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="35">
   <si>
     <t>method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -137,6 +137,14 @@
   </si>
   <si>
     <t>Graph size:  17903 197031</t>
+  </si>
+  <si>
+    <t>GSBA_old_RC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GSBA_old_JC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -532,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R67"/>
+  <dimension ref="A1:R73"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="M67" activeCellId="2" sqref="M55:R60 M64:R64 M67:R67"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="T71" sqref="T71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1305,2248 +1313,2576 @@
         <v>0.56799999999999995</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B21" s="4" t="s">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>0.44</v>
+      </c>
+      <c r="E19">
+        <v>0.43</v>
+      </c>
+      <c r="F19">
+        <v>0.4</v>
+      </c>
+      <c r="G19">
+        <v>0.39</v>
+      </c>
+      <c r="H19">
+        <v>0.38</v>
+      </c>
+      <c r="I19">
+        <v>0.4</v>
+      </c>
+      <c r="M19">
+        <v>0.46</v>
+      </c>
+      <c r="N19">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="O19">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="P19">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="Q19">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="R19">
+        <v>0.378</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>0.39</v>
+      </c>
+      <c r="E20">
+        <v>0.38</v>
+      </c>
+      <c r="F20">
+        <v>0.43</v>
+      </c>
+      <c r="G20">
+        <v>0.37</v>
+      </c>
+      <c r="H20">
+        <v>0.31</v>
+      </c>
+      <c r="I20">
+        <v>0.35</v>
+      </c>
+      <c r="M20">
+        <v>0.432</v>
+      </c>
+      <c r="N20">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="O20">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="P20">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="Q20">
+        <v>0.35</v>
+      </c>
+      <c r="R20">
+        <v>0.33600000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="B22" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:18" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:18" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B23" s="3">
         <v>3</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C23" s="3">
         <v>4</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D23" s="3">
         <v>5</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E23" s="3">
         <v>6</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F23" s="3">
         <v>7</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G23" s="3">
         <v>8</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H23" s="3">
         <v>9</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I23" s="3">
         <v>10</v>
       </c>
-      <c r="J22" s="5"/>
-      <c r="K22" s="3">
+      <c r="J23" s="5"/>
+      <c r="K23" s="3">
         <v>3</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L23" s="3">
         <v>4</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M23" s="3">
         <v>5</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N23" s="3">
         <v>6</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O23" s="3">
         <v>7</v>
       </c>
-      <c r="P22" s="3">
+      <c r="P23" s="3">
         <v>8</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="Q23" s="3">
         <v>9</v>
       </c>
-      <c r="R22" s="3">
+      <c r="R23" s="3">
         <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <v>0.25907415782587301</v>
-      </c>
-      <c r="C23">
-        <v>0.29617624039596802</v>
-      </c>
-      <c r="D23">
-        <v>0.42427212234286299</v>
-      </c>
-      <c r="E23">
-        <v>0.48210410709596002</v>
-      </c>
-      <c r="F23">
-        <v>0.494685010986185</v>
-      </c>
-      <c r="G23">
-        <v>0.49576765906569498</v>
-      </c>
-      <c r="H23">
-        <v>0.60274787911123895</v>
-      </c>
-      <c r="I23">
-        <v>0.68312189600276496</v>
-      </c>
-      <c r="K23">
-        <v>0.22295309823452999</v>
-      </c>
-      <c r="L23">
-        <v>0.353101759601188</v>
-      </c>
-      <c r="M23">
-        <v>0.43285750356422298</v>
-      </c>
-      <c r="N23">
-        <v>0.47733347883448701</v>
-      </c>
-      <c r="O23">
-        <v>0.50547837912017302</v>
-      </c>
-      <c r="P23">
-        <v>0.54807935061817603</v>
-      </c>
-      <c r="Q23">
-        <v>0.54842579213940101</v>
-      </c>
-      <c r="R23">
-        <v>0.59664144168975997</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24">
-        <v>0.26584014652063398</v>
+        <v>0.25907415782587301</v>
       </c>
       <c r="C24">
-        <v>0.28732269415297901</v>
+        <v>0.29617624039596802</v>
       </c>
       <c r="D24">
-        <v>0.420775937777144</v>
+        <v>0.42427212234286299</v>
       </c>
       <c r="E24">
-        <v>0.459352975894249</v>
+        <v>0.48210410709596002</v>
       </c>
       <c r="F24">
         <v>0.494685010986185</v>
       </c>
       <c r="G24">
-        <v>0.49197256009401202</v>
+        <v>0.49576765906569498</v>
       </c>
       <c r="H24">
-        <v>0.62595643924646804</v>
+        <v>0.60274787911123895</v>
       </c>
       <c r="I24">
-        <v>0.68227433371324697</v>
+        <v>0.68312189600276496</v>
       </c>
       <c r="K24">
-        <v>0.22263083676770701</v>
+        <v>0.22295309823452999</v>
       </c>
       <c r="L24">
-        <v>0.33476938470597201</v>
+        <v>0.353101759601188</v>
       </c>
       <c r="M24">
-        <v>0.43055386616922398</v>
+        <v>0.43285750356422298</v>
       </c>
       <c r="N24">
-        <v>0.47360415920601601</v>
+        <v>0.47733347883448701</v>
       </c>
       <c r="O24">
-        <v>0.51159585783375106</v>
+        <v>0.50547837912017302</v>
       </c>
       <c r="P24">
-        <v>0.54823638011433495</v>
+        <v>0.54807935061817603</v>
       </c>
       <c r="Q24">
-        <v>0.55607138831963898</v>
+        <v>0.54842579213940101</v>
       </c>
       <c r="R24">
-        <v>0.59057875440340901</v>
+        <v>0.59664144168975997</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25">
         <v>0.26584014652063398</v>
       </c>
       <c r="C25">
-        <v>0.37511399247858102</v>
+        <v>0.28732269415297901</v>
       </c>
       <c r="D25">
-        <v>0.482985601437593</v>
+        <v>0.420775937777144</v>
       </c>
       <c r="E25">
-        <v>0.491692156535327</v>
+        <v>0.459352975894249</v>
       </c>
       <c r="F25">
-        <v>0.48191281603254099</v>
+        <v>0.494685010986185</v>
       </c>
       <c r="G25">
-        <v>0.53315666533102102</v>
+        <v>0.49197256009401202</v>
       </c>
       <c r="H25">
-        <v>0.53537721871912902</v>
+        <v>0.62595643924646804</v>
       </c>
       <c r="I25">
-        <v>0.59172568005805604</v>
+        <v>0.68227433371324697</v>
       </c>
       <c r="K25">
         <v>0.22263083676770701</v>
       </c>
       <c r="L25">
-        <v>0.35175013768882102</v>
+        <v>0.33476938470597201</v>
       </c>
       <c r="M25">
-        <v>0.44662048468636301</v>
+        <v>0.43055386616922398</v>
       </c>
       <c r="N25">
-        <v>0.47448302108053803</v>
+        <v>0.47360415920601601</v>
       </c>
       <c r="O25">
-        <v>0.48167408048271998</v>
+        <v>0.51159585783375106</v>
       </c>
       <c r="P25">
-        <v>0.52409949208084605</v>
+        <v>0.54823638011433495</v>
       </c>
       <c r="Q25">
-        <v>0.47344888605907098</v>
+        <v>0.55607138831963898</v>
       </c>
       <c r="R25">
-        <v>0.51734692994198805</v>
+        <v>0.59057875440340901</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26">
-        <v>0.25907415782587301</v>
+        <v>0.26584014652063398</v>
       </c>
       <c r="C26">
-        <v>0.27629019231386298</v>
+        <v>0.37511399247858102</v>
       </c>
       <c r="D26">
-        <v>0.42949708988983398</v>
+        <v>0.482985601437593</v>
       </c>
       <c r="E26">
-        <v>0.48769463472284302</v>
+        <v>0.491692156535327</v>
       </c>
       <c r="F26">
-        <v>0.49852228948699101</v>
+        <v>0.48191281603254099</v>
       </c>
       <c r="G26">
-        <v>0.50352169702676597</v>
+        <v>0.53315666533102102</v>
       </c>
       <c r="H26">
-        <v>0.624495533964188</v>
+        <v>0.53537721871912902</v>
       </c>
       <c r="I26">
-        <v>0.724358097937153</v>
+        <v>0.59172568005805604</v>
       </c>
       <c r="K26">
-        <v>0.22295309823452999</v>
+        <v>0.22263083676770701</v>
       </c>
       <c r="L26">
-        <v>0.34655495915929102</v>
+        <v>0.35175013768882102</v>
       </c>
       <c r="M26">
-        <v>0.43061739482896599</v>
+        <v>0.44662048468636301</v>
       </c>
       <c r="N26">
-        <v>0.47753604439828101</v>
+        <v>0.47448302108053803</v>
       </c>
       <c r="O26">
-        <v>0.52431684869346495</v>
+        <v>0.48167408048271998</v>
       </c>
       <c r="P26">
-        <v>0.56945805784438297</v>
+        <v>0.52409949208084605</v>
       </c>
       <c r="Q26">
-        <v>0.56615499456910601</v>
+        <v>0.47344888605907098</v>
       </c>
       <c r="R26">
-        <v>0.60203855292020203</v>
+        <v>0.51734692994198805</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>0.24158275364960399</v>
+        <v>0.25907415782587301</v>
       </c>
       <c r="C27">
-        <v>0.38444149469793398</v>
+        <v>0.27629019231386298</v>
       </c>
       <c r="D27">
-        <v>0.498316623632311</v>
+        <v>0.42949708988983398</v>
       </c>
       <c r="E27">
-        <v>0.54853165646602198</v>
+        <v>0.48769463472284302</v>
       </c>
       <c r="F27">
-        <v>0.53204727528133799</v>
+        <v>0.49852228948699101</v>
       </c>
       <c r="G27">
-        <v>0.52381003557769001</v>
+        <v>0.50352169702676597</v>
       </c>
       <c r="H27">
-        <v>0.65077981728119305</v>
+        <v>0.624495533964188</v>
       </c>
       <c r="I27">
-        <v>0.74227855554145705</v>
+        <v>0.724358097937153</v>
       </c>
       <c r="K27">
-        <v>0.228041992671316</v>
+        <v>0.22295309823452999</v>
       </c>
       <c r="L27">
-        <v>0.35757879211773902</v>
+        <v>0.34655495915929102</v>
       </c>
       <c r="M27">
-        <v>0.46065475963040098</v>
+        <v>0.43061739482896599</v>
       </c>
       <c r="N27">
-        <v>0.52797460588118506</v>
+        <v>0.47753604439828101</v>
       </c>
       <c r="O27">
-        <v>0.55501213463577403</v>
+        <v>0.52431684869346495</v>
       </c>
       <c r="P27">
-        <v>0.598166055260965</v>
+        <v>0.56945805784438297</v>
       </c>
       <c r="Q27">
-        <v>0.62661690971114903</v>
+        <v>0.56615499456910601</v>
       </c>
       <c r="R27">
-        <v>0.68029024389095005</v>
+        <v>0.60203855292020203</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28">
-        <v>0.164732237516654</v>
+        <v>0.24158275364960399</v>
       </c>
       <c r="C28">
-        <v>0.22196640176858301</v>
+        <v>0.38444149469793398</v>
       </c>
       <c r="D28">
-        <v>0.318725919072952</v>
+        <v>0.498316623632311</v>
       </c>
       <c r="E28">
-        <v>0.273707414568788</v>
+        <v>0.54853165646602198</v>
       </c>
       <c r="F28">
-        <v>0.33749646415341</v>
+        <v>0.53204727528133799</v>
       </c>
       <c r="G28">
-        <v>0.33686696657356102</v>
+        <v>0.52381003557769001</v>
       </c>
       <c r="H28">
-        <v>0.30464256635547798</v>
+        <v>0.65077981728119305</v>
       </c>
       <c r="I28">
-        <v>0.39750182922166299</v>
+        <v>0.74227855554145705</v>
       </c>
       <c r="K28">
-        <v>0.16852656355791201</v>
+        <v>0.228041992671316</v>
       </c>
       <c r="L28">
-        <v>0.20935573281216499</v>
+        <v>0.35757879211773902</v>
       </c>
       <c r="M28">
-        <v>0.27736494233995002</v>
+        <v>0.46065475963040098</v>
       </c>
       <c r="N28">
-        <v>0.28887183313416798</v>
+        <v>0.52797460588118506</v>
       </c>
       <c r="O28">
-        <v>0.31109406279562202</v>
+        <v>0.55501213463577403</v>
       </c>
       <c r="P28">
-        <v>0.31589685873416701</v>
+        <v>0.598166055260965</v>
       </c>
       <c r="Q28">
-        <v>0.31888792279593298</v>
+        <v>0.62661690971114903</v>
       </c>
       <c r="R28">
-        <v>0.36006600389917498</v>
+        <v>0.68029024389095005</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29">
-        <v>0.255175707440295</v>
+        <v>0.164732237516654</v>
       </c>
       <c r="C29">
-        <v>0.31471663700817598</v>
+        <v>0.22196640176858301</v>
       </c>
       <c r="D29">
-        <v>0.35157350129623999</v>
+        <v>0.318725919072952</v>
       </c>
       <c r="E29">
-        <v>0.39601895464256698</v>
+        <v>0.273707414568788</v>
       </c>
       <c r="F29">
-        <v>0.38171011599031401</v>
+        <v>0.33749646415341</v>
       </c>
       <c r="G29">
-        <v>0.33072653012458803</v>
+        <v>0.33686696657356102</v>
       </c>
       <c r="H29">
-        <v>0.47518142484326698</v>
+        <v>0.30464256635547798</v>
       </c>
       <c r="I29">
-        <v>0.533497649656555</v>
+        <v>0.39750182922166299</v>
       </c>
       <c r="K29">
-        <v>0.20918578068787999</v>
+        <v>0.16852656355791201</v>
       </c>
       <c r="L29">
-        <v>0.258584026489107</v>
+        <v>0.20935573281216499</v>
       </c>
       <c r="M29">
-        <v>0.352563443829635</v>
+        <v>0.27736494233995002</v>
       </c>
       <c r="N29">
-        <v>0.37970350130936298</v>
+        <v>0.28887183313416798</v>
       </c>
       <c r="O29">
-        <v>0.38512435316819199</v>
+        <v>0.31109406279562202</v>
       </c>
       <c r="P29">
-        <v>0.46526228554027699</v>
+        <v>0.31589685873416701</v>
       </c>
       <c r="Q29">
-        <v>0.44614200332034898</v>
+        <v>0.31888792279593298</v>
       </c>
       <c r="R29">
-        <v>0.48204115089227501</v>
+        <v>0.36006600389917498</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30">
-        <v>0.21000911896114399</v>
+        <v>0.255175707440295</v>
       </c>
       <c r="C30">
-        <v>0.227344871370215</v>
+        <v>0.31471663700817598</v>
       </c>
       <c r="D30">
-        <v>0.30672015686694398</v>
+        <v>0.35157350129623999</v>
       </c>
       <c r="E30">
-        <v>0.27713420785415499</v>
+        <v>0.39601895464256698</v>
       </c>
       <c r="F30">
-        <v>0.36476795184116201</v>
+        <v>0.38171011599031401</v>
       </c>
       <c r="G30">
-        <v>0.34848994386156001</v>
+        <v>0.33072653012458803</v>
       </c>
       <c r="H30">
-        <v>0.38237567152298901</v>
+        <v>0.47518142484326698</v>
       </c>
       <c r="I30">
-        <v>0.54550622821856198</v>
+        <v>0.533497649656555</v>
       </c>
       <c r="K30">
-        <v>0.175196191625311</v>
+        <v>0.20918578068787999</v>
       </c>
       <c r="L30">
-        <v>0.200520769913309</v>
+        <v>0.258584026489107</v>
       </c>
       <c r="M30">
-        <v>0.277176290046526</v>
+        <v>0.352563443829635</v>
       </c>
       <c r="N30">
-        <v>0.31755176743825397</v>
+        <v>0.37970350130936298</v>
       </c>
       <c r="O30">
-        <v>0.35362492859211397</v>
+        <v>0.38512435316819199</v>
       </c>
       <c r="P30">
-        <v>0.38058283535924797</v>
+        <v>0.46526228554027699</v>
       </c>
       <c r="Q30">
-        <v>0.36514942305623499</v>
+        <v>0.44614200332034898</v>
       </c>
       <c r="R30">
-        <v>0.43694384696862498</v>
+        <v>0.48204115089227501</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31">
-        <v>0.217198700882139</v>
+        <v>0.21000911896114399</v>
       </c>
       <c r="C31">
-        <v>0.28505287442457</v>
+        <v>0.227344871370215</v>
       </c>
       <c r="D31">
-        <v>0.32836468996303197</v>
+        <v>0.30672015686694398</v>
       </c>
       <c r="E31">
-        <v>0.39728997368225699</v>
+        <v>0.27713420785415499</v>
       </c>
       <c r="F31">
-        <v>0.380757511226544</v>
+        <v>0.36476795184116201</v>
       </c>
       <c r="G31">
-        <v>0.39396981907354101</v>
+        <v>0.34848994386156001</v>
       </c>
       <c r="H31">
-        <v>0.45086469328865902</v>
+        <v>0.38237567152298901</v>
       </c>
       <c r="I31">
-        <v>0.54497247967457196</v>
+        <v>0.54550622821856198</v>
       </c>
       <c r="K31">
-        <v>0.19295334118096899</v>
+        <v>0.175196191625311</v>
       </c>
       <c r="L31">
-        <v>0.22501887129463299</v>
+        <v>0.200520769913309</v>
       </c>
       <c r="M31">
-        <v>0.32518522633361902</v>
+        <v>0.277176290046526</v>
       </c>
       <c r="N31">
-        <v>0.36733854142703198</v>
+        <v>0.31755176743825397</v>
       </c>
       <c r="O31">
-        <v>0.39273044110250699</v>
+        <v>0.35362492859211397</v>
       </c>
       <c r="P31">
-        <v>0.44760046748579801</v>
+        <v>0.38058283535924797</v>
       </c>
       <c r="Q31">
-        <v>0.43237749804937498</v>
+        <v>0.36514942305623499</v>
       </c>
       <c r="R31">
-        <v>0.478659788319102</v>
+        <v>0.43694384696862498</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32">
-        <v>0.21368644861203601</v>
+        <v>0.217198700882139</v>
       </c>
       <c r="C32">
-        <v>0.29522665648213697</v>
+        <v>0.28505287442457</v>
       </c>
       <c r="D32">
-        <v>0.33122913247992702</v>
+        <v>0.32836468996303197</v>
       </c>
       <c r="E32">
-        <v>0.40646634787268998</v>
+        <v>0.39728997368225699</v>
       </c>
       <c r="F32">
-        <v>0.37042439778882003</v>
+        <v>0.380757511226544</v>
       </c>
       <c r="G32">
-        <v>0.34684980515529601</v>
+        <v>0.39396981907354101</v>
       </c>
       <c r="H32">
-        <v>0.42386646947937101</v>
+        <v>0.45086469328865902</v>
       </c>
       <c r="I32">
-        <v>0.52696315623219603</v>
+        <v>0.54497247967457196</v>
       </c>
       <c r="K32">
-        <v>0.177357241852859</v>
+        <v>0.19295334118096899</v>
       </c>
       <c r="L32">
-        <v>0.22810850049943601</v>
+        <v>0.22501887129463299</v>
       </c>
       <c r="M32">
-        <v>0.31093243334873299</v>
+        <v>0.32518522633361902</v>
       </c>
       <c r="N32">
-        <v>0.36817966411387498</v>
+        <v>0.36733854142703198</v>
       </c>
       <c r="O32">
-        <v>0.38917383581939202</v>
+        <v>0.39273044110250699</v>
       </c>
       <c r="P32">
-        <v>0.44352249993995502</v>
+        <v>0.44760046748579801</v>
       </c>
       <c r="Q32">
-        <v>0.41907064793360099</v>
+        <v>0.43237749804937498</v>
       </c>
       <c r="R32">
-        <v>0.47852481801014202</v>
+        <v>0.478659788319102</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33">
-        <v>0.22599748407152101</v>
+        <v>0.21368644861203601</v>
       </c>
       <c r="C33">
-        <v>0.28505287442457</v>
+        <v>0.29522665648213697</v>
       </c>
       <c r="D33">
-        <v>0.31504181942246801</v>
+        <v>0.33122913247992702</v>
       </c>
       <c r="E33">
-        <v>0.39728997368225699</v>
+        <v>0.40646634787268998</v>
       </c>
       <c r="F33">
-        <v>0.37034812635394798</v>
+        <v>0.37042439778882003</v>
       </c>
       <c r="G33">
-        <v>0.38327793533005999</v>
+        <v>0.34684980515529601</v>
       </c>
       <c r="H33">
-        <v>0.441584357378771</v>
+        <v>0.42386646947937101</v>
       </c>
       <c r="I33">
-        <v>0.54497247967457196</v>
+        <v>0.52696315623219603</v>
       </c>
       <c r="K33">
-        <v>0.197232710593017</v>
+        <v>0.177357241852859</v>
       </c>
       <c r="L33">
-        <v>0.22535810131171599</v>
+        <v>0.22810850049943601</v>
       </c>
       <c r="M33">
-        <v>0.32251638156904799</v>
+        <v>0.31093243334873299</v>
       </c>
       <c r="N33">
-        <v>0.36767968194477602</v>
+        <v>0.36817966411387498</v>
       </c>
       <c r="O33">
-        <v>0.39412585441002101</v>
+        <v>0.38917383581939202</v>
       </c>
       <c r="P33">
-        <v>0.44706934699763601</v>
+        <v>0.44352249993995502</v>
       </c>
       <c r="Q33">
-        <v>0.43135054880198898</v>
+        <v>0.41907064793360099</v>
       </c>
       <c r="R33">
-        <v>0.47846319948676203</v>
+        <v>0.47852481801014202</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34">
-        <v>0.14931991085388699</v>
+        <v>0.22599748407152101</v>
       </c>
       <c r="C34">
-        <v>0.22196640176858301</v>
+        <v>0.28505287442457</v>
       </c>
       <c r="D34">
-        <v>0.322205449449532</v>
+        <v>0.31504181942246801</v>
       </c>
       <c r="E34">
-        <v>0.273707414568788</v>
+        <v>0.39728997368225699</v>
       </c>
       <c r="F34">
-        <v>0.32335424685613601</v>
+        <v>0.37034812635394798</v>
       </c>
       <c r="G34">
-        <v>0.34675113044668598</v>
+        <v>0.38327793533005999</v>
       </c>
       <c r="H34">
-        <v>0.30464256635547798</v>
+        <v>0.441584357378771</v>
       </c>
       <c r="I34">
-        <v>0.40468014118409901</v>
+        <v>0.54497247967457196</v>
       </c>
       <c r="K34">
-        <v>0.167008477803613</v>
+        <v>0.197232710593017</v>
       </c>
       <c r="L34">
-        <v>0.20665009458165501</v>
+        <v>0.22535810131171599</v>
       </c>
       <c r="M34">
-        <v>0.278764789016617</v>
+        <v>0.32251638156904799</v>
       </c>
       <c r="N34">
-        <v>0.286364075963491</v>
+        <v>0.36767968194477602</v>
       </c>
       <c r="O34">
-        <v>0.30155336498955398</v>
+        <v>0.39412585441002101</v>
       </c>
       <c r="P34">
-        <v>0.314543430588485</v>
+        <v>0.44706934699763601</v>
       </c>
       <c r="Q34">
-        <v>0.31633991150229102</v>
+        <v>0.43135054880198898</v>
       </c>
       <c r="R34">
-        <v>0.35038847093476599</v>
+        <v>0.47846319948676203</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <v>0.14931991085388699</v>
+      </c>
+      <c r="C35">
+        <v>0.22196640176858301</v>
+      </c>
+      <c r="D35">
+        <v>0.322205449449532</v>
+      </c>
+      <c r="E35">
+        <v>0.273707414568788</v>
+      </c>
+      <c r="F35">
+        <v>0.32335424685613601</v>
+      </c>
+      <c r="G35">
+        <v>0.34675113044668598</v>
+      </c>
+      <c r="H35">
+        <v>0.30464256635547798</v>
+      </c>
+      <c r="I35">
+        <v>0.40468014118409901</v>
+      </c>
+      <c r="K35">
+        <v>0.167008477803613</v>
+      </c>
+      <c r="L35">
+        <v>0.20665009458165501</v>
+      </c>
+      <c r="M35">
+        <v>0.278764789016617</v>
+      </c>
+      <c r="N35">
+        <v>0.286364075963491</v>
+      </c>
+      <c r="O35">
+        <v>0.30155336498955398</v>
+      </c>
+      <c r="P35">
+        <v>0.314543430588485</v>
+      </c>
+      <c r="Q35">
+        <v>0.31633991150229102</v>
+      </c>
+      <c r="R35">
+        <v>0.35038847093476599</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
         <v>29</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>0.17896835318028601</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>0.245226728210094</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <v>0.29109340204105799</v>
       </c>
-      <c r="E35">
+      <c r="E36">
         <v>0.31940855454636502</v>
       </c>
-      <c r="F35">
+      <c r="F36">
         <v>0.25563117677054897</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <v>0.27994653543664599</v>
       </c>
-      <c r="H35">
+      <c r="H36">
         <v>0.31841840868398902</v>
       </c>
-      <c r="I35">
+      <c r="I36">
         <v>0.42529300562029698</v>
       </c>
-      <c r="K35">
+      <c r="K36">
         <v>0.16677198749842501</v>
       </c>
-      <c r="L35">
+      <c r="L36">
         <v>0.20924224745225301</v>
       </c>
-      <c r="M35">
+      <c r="M36">
         <v>0.263719390962317</v>
       </c>
-      <c r="N35">
+      <c r="N36">
         <v>0.28666237398734501</v>
       </c>
-      <c r="O35">
+      <c r="O36">
         <v>0.31396927636076599</v>
       </c>
-      <c r="P35">
+      <c r="P36">
         <v>0.30908007270176802</v>
       </c>
-      <c r="Q35">
+      <c r="Q36">
         <v>0.293849262367679</v>
       </c>
-      <c r="R35">
+      <c r="R36">
         <v>0.33253433608627198</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B37" s="4" t="s">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37">
+        <v>0.3911</v>
+      </c>
+      <c r="E37">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="F37">
+        <v>0.433</v>
+      </c>
+      <c r="G37">
+        <v>0.45450000000000002</v>
+      </c>
+      <c r="H37">
+        <v>0.49469999999999997</v>
+      </c>
+      <c r="I37">
+        <v>0.51859999999999995</v>
+      </c>
+      <c r="M37">
+        <v>0.35120000000000001</v>
+      </c>
+      <c r="N37">
+        <v>0.39319999999999999</v>
+      </c>
+      <c r="O37">
+        <v>0.44629999999999997</v>
+      </c>
+      <c r="P37">
+        <v>0.46560000000000001</v>
+      </c>
+      <c r="Q37">
+        <v>0.46089999999999998</v>
+      </c>
+      <c r="R37">
+        <v>0.4743</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38">
+        <v>0.42270000000000002</v>
+      </c>
+      <c r="E38">
+        <v>0.46150000000000002</v>
+      </c>
+      <c r="F38">
+        <v>0.43869999999999998</v>
+      </c>
+      <c r="G38">
+        <v>0.57040000000000002</v>
+      </c>
+      <c r="H38">
+        <v>0.65229999999999999</v>
+      </c>
+      <c r="I38">
+        <v>0.63419999999999999</v>
+      </c>
+      <c r="M38">
+        <v>0.38429999999999997</v>
+      </c>
+      <c r="N38">
+        <v>0.44990000000000002</v>
+      </c>
+      <c r="O38">
+        <v>0.53120000000000001</v>
+      </c>
+      <c r="P38">
+        <v>0.58889999999999998</v>
+      </c>
+      <c r="Q38">
+        <v>0.61639999999999995</v>
+      </c>
+      <c r="R38">
+        <v>0.60840000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="B40" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:18" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="1" t="s">
+    <row r="41" spans="1:18" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B41" s="3">
         <v>3</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C41" s="3">
         <v>4</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D41" s="3">
         <v>5</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E41" s="3">
         <v>6</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F41" s="3">
         <v>7</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G41" s="3">
         <v>8</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H41" s="3">
         <v>9</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I41" s="3">
         <v>10</v>
       </c>
-      <c r="J38" s="5"/>
-      <c r="K38" s="3">
+      <c r="J41" s="5"/>
+      <c r="K41" s="3">
         <v>3</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L41" s="3">
         <v>4</v>
       </c>
-      <c r="M38" s="3">
+      <c r="M41" s="3">
         <v>5</v>
       </c>
-      <c r="N38" s="3">
+      <c r="N41" s="3">
         <v>6</v>
       </c>
-      <c r="O38" s="3">
+      <c r="O41" s="3">
         <v>7</v>
       </c>
-      <c r="P38" s="3">
+      <c r="P41" s="3">
         <v>8</v>
       </c>
-      <c r="Q38" s="3">
+      <c r="Q41" s="3">
         <v>9</v>
       </c>
-      <c r="R38" s="3">
+      <c r="R41" s="3">
         <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39">
-        <v>0.42</v>
-      </c>
-      <c r="C39">
-        <v>0.53</v>
-      </c>
-      <c r="D39">
-        <v>0.7</v>
-      </c>
-      <c r="E39">
-        <v>0.82</v>
-      </c>
-      <c r="F39">
-        <v>0.8</v>
-      </c>
-      <c r="G39">
-        <v>0.84</v>
-      </c>
-      <c r="H39">
-        <v>0.98</v>
-      </c>
-      <c r="I39">
-        <v>1.04</v>
-      </c>
-      <c r="K39">
-        <v>0.374</v>
-      </c>
-      <c r="L39">
-        <v>0.59</v>
-      </c>
-      <c r="M39">
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="N39">
-        <v>0.79600000000000004</v>
-      </c>
-      <c r="O39">
-        <v>0.83199999999999996</v>
-      </c>
-      <c r="P39">
-        <v>0.88600000000000001</v>
-      </c>
-      <c r="Q39">
-        <v>0.90800000000000003</v>
-      </c>
-      <c r="R39">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40">
-        <v>0.43</v>
-      </c>
-      <c r="C40">
-        <v>0.52</v>
-      </c>
-      <c r="D40">
-        <v>0.69</v>
-      </c>
-      <c r="E40">
-        <v>0.76</v>
-      </c>
-      <c r="F40">
-        <v>0.8</v>
-      </c>
-      <c r="G40">
-        <v>0.82</v>
-      </c>
-      <c r="H40">
-        <v>1.01</v>
-      </c>
-      <c r="I40">
-        <v>1.03</v>
-      </c>
-      <c r="K40">
-        <v>0.374</v>
-      </c>
-      <c r="L40">
-        <v>0.56399999999999995</v>
-      </c>
-      <c r="M40">
-        <v>0.71799999999999997</v>
-      </c>
-      <c r="N40">
-        <v>0.79200000000000004</v>
-      </c>
-      <c r="O40">
-        <v>0.84599999999999997</v>
-      </c>
-      <c r="P40">
-        <v>0.89400000000000002</v>
-      </c>
-      <c r="Q40">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="R40">
-        <v>0.99399999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41">
-        <v>0.43</v>
-      </c>
-      <c r="C41">
-        <v>0.64</v>
-      </c>
-      <c r="D41">
-        <v>0.78</v>
-      </c>
-      <c r="E41">
-        <v>0.8</v>
-      </c>
-      <c r="F41">
-        <v>0.8</v>
-      </c>
-      <c r="G41">
-        <v>0.91</v>
-      </c>
-      <c r="H41">
-        <v>0.87</v>
-      </c>
-      <c r="I41">
-        <v>0.93</v>
-      </c>
-      <c r="K41">
-        <v>0.374</v>
-      </c>
-      <c r="L41">
-        <v>0.59799999999999998</v>
-      </c>
-      <c r="M41">
-        <v>0.74</v>
-      </c>
-      <c r="N41">
-        <v>0.79200000000000004</v>
-      </c>
-      <c r="O41">
-        <v>0.79200000000000004</v>
-      </c>
-      <c r="P41">
-        <v>0.85599999999999998</v>
-      </c>
-      <c r="Q41">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="R41">
-        <v>0.88400000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B42">
         <v>0.42</v>
       </c>
       <c r="C42">
-        <v>0.51</v>
+        <v>0.53</v>
       </c>
       <c r="D42">
-        <v>0.72</v>
+        <v>0.7</v>
       </c>
       <c r="E42">
-        <v>0.83</v>
+        <v>0.82</v>
       </c>
       <c r="F42">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
       <c r="G42">
-        <v>0.85</v>
+        <v>0.84</v>
       </c>
       <c r="H42">
-        <v>1.02</v>
+        <v>0.98</v>
       </c>
       <c r="I42">
-        <v>1.1399999999999999</v>
+        <v>1.04</v>
       </c>
       <c r="K42">
         <v>0.374</v>
       </c>
       <c r="L42">
-        <v>0.58599999999999997</v>
+        <v>0.59</v>
       </c>
       <c r="M42">
-        <v>0.71799999999999997</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="N42">
-        <v>0.80400000000000005</v>
+        <v>0.79600000000000004</v>
       </c>
       <c r="O42">
-        <v>0.874</v>
+        <v>0.83199999999999996</v>
       </c>
       <c r="P42">
-        <v>0.93400000000000005</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="Q42">
-        <v>0.96399999999999997</v>
+        <v>0.90800000000000003</v>
       </c>
       <c r="R42">
-        <v>1.022</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B43">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="C43">
-        <v>0.65</v>
+        <v>0.52</v>
       </c>
       <c r="D43">
-        <v>0.81</v>
+        <v>0.69</v>
       </c>
       <c r="E43">
-        <v>0.89</v>
+        <v>0.76</v>
       </c>
       <c r="F43">
-        <v>0.87</v>
+        <v>0.8</v>
       </c>
       <c r="G43">
-        <v>0.9</v>
+        <v>0.82</v>
       </c>
       <c r="H43">
-        <v>1.06</v>
+        <v>1.01</v>
       </c>
       <c r="I43">
-        <v>1.1299999999999999</v>
+        <v>1.03</v>
       </c>
       <c r="K43">
-        <v>0.378</v>
+        <v>0.374</v>
       </c>
       <c r="L43">
-        <v>0.6</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="M43">
-        <v>0.752</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="N43">
-        <v>0.86</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="O43">
-        <v>0.90400000000000003</v>
+        <v>0.84599999999999997</v>
       </c>
       <c r="P43">
-        <v>0.96199999999999997</v>
+        <v>0.89400000000000002</v>
       </c>
       <c r="Q43">
-        <v>1.024</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="R43">
-        <v>1.1060000000000001</v>
+        <v>0.99399999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B44">
-        <v>0.26</v>
+        <v>0.43</v>
       </c>
       <c r="C44">
-        <v>0.38</v>
+        <v>0.64</v>
       </c>
       <c r="D44">
-        <v>0.49</v>
+        <v>0.78</v>
       </c>
       <c r="E44">
-        <v>0.43</v>
+        <v>0.8</v>
       </c>
       <c r="F44">
-        <v>0.51</v>
+        <v>0.8</v>
       </c>
       <c r="G44">
-        <v>0.62</v>
+        <v>0.91</v>
       </c>
       <c r="H44">
-        <v>0.52</v>
+        <v>0.87</v>
       </c>
       <c r="I44">
-        <v>0.61</v>
+        <v>0.93</v>
       </c>
       <c r="K44">
-        <v>0.27200000000000002</v>
+        <v>0.374</v>
       </c>
       <c r="L44">
-        <v>0.34</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="M44">
-        <v>0.438</v>
+        <v>0.74</v>
       </c>
       <c r="N44">
-        <v>0.47399999999999998</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="O44">
-        <v>0.51</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="P44">
-        <v>0.52</v>
+        <v>0.85599999999999998</v>
       </c>
       <c r="Q44">
-        <v>0.53200000000000003</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="R44">
-        <v>0.60799999999999998</v>
+        <v>0.88400000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B45">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="C45">
-        <v>0.49</v>
+        <v>0.51</v>
       </c>
       <c r="D45">
-        <v>0.59</v>
+        <v>0.72</v>
       </c>
       <c r="E45">
-        <v>0.63</v>
+        <v>0.83</v>
       </c>
       <c r="F45">
-        <v>0.67</v>
+        <v>0.82</v>
       </c>
       <c r="G45">
-        <v>0.57999999999999996</v>
+        <v>0.85</v>
       </c>
       <c r="H45">
-        <v>0.81</v>
+        <v>1.02</v>
       </c>
       <c r="I45">
-        <v>0.91</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="K45">
-        <v>0.34399999999999997</v>
+        <v>0.374</v>
       </c>
       <c r="L45">
-        <v>0.442</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="M45">
-        <v>0.57799999999999996</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="N45">
-        <v>0.65800000000000003</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="O45">
-        <v>0.67400000000000004</v>
+        <v>0.874</v>
       </c>
       <c r="P45">
-        <v>0.79200000000000004</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="Q45">
-        <v>0.80200000000000005</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="R45">
-        <v>0.89</v>
+        <v>1.022</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B46">
-        <v>0.33</v>
+        <v>0.4</v>
       </c>
       <c r="C46">
-        <v>0.35</v>
+        <v>0.65</v>
       </c>
       <c r="D46">
-        <v>0.49</v>
+        <v>0.81</v>
       </c>
       <c r="E46">
-        <v>0.39</v>
+        <v>0.89</v>
       </c>
       <c r="F46">
-        <v>0.56999999999999995</v>
+        <v>0.87</v>
       </c>
       <c r="G46">
-        <v>0.61</v>
+        <v>0.9</v>
       </c>
       <c r="H46">
-        <v>0.61</v>
+        <v>1.06</v>
       </c>
       <c r="I46">
-        <v>0.84</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="K46">
-        <v>0.27800000000000002</v>
+        <v>0.378</v>
       </c>
       <c r="L46">
-        <v>0.33200000000000002</v>
+        <v>0.6</v>
       </c>
       <c r="M46">
-        <v>0.42799999999999999</v>
+        <v>0.752</v>
       </c>
       <c r="N46">
-        <v>0.50800000000000001</v>
+        <v>0.86</v>
       </c>
       <c r="O46">
-        <v>0.56599999999999995</v>
+        <v>0.90400000000000003</v>
       </c>
       <c r="P46">
-        <v>0.6</v>
+        <v>0.96199999999999997</v>
       </c>
       <c r="Q46">
-        <v>0.59399999999999997</v>
+        <v>1.024</v>
       </c>
       <c r="R46">
-        <v>0.72799999999999998</v>
+        <v>1.1060000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B47">
-        <v>0.35</v>
+        <v>0.26</v>
       </c>
       <c r="C47">
-        <v>0.44</v>
+        <v>0.38</v>
       </c>
       <c r="D47">
-        <v>0.54</v>
+        <v>0.49</v>
       </c>
       <c r="E47">
-        <v>0.63</v>
+        <v>0.43</v>
       </c>
       <c r="F47">
-        <v>0.65</v>
+        <v>0.51</v>
       </c>
       <c r="G47">
-        <v>0.67</v>
+        <v>0.62</v>
       </c>
       <c r="H47">
-        <v>0.77</v>
+        <v>0.52</v>
       </c>
       <c r="I47">
-        <v>0.94</v>
+        <v>0.61</v>
       </c>
       <c r="K47">
-        <v>0.316</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="L47">
-        <v>0.39</v>
+        <v>0.34</v>
       </c>
       <c r="M47">
-        <v>0.53400000000000003</v>
+        <v>0.438</v>
       </c>
       <c r="N47">
-        <v>0.63</v>
+        <v>0.47399999999999998</v>
       </c>
       <c r="O47">
-        <v>0.69399999999999995</v>
+        <v>0.51</v>
       </c>
       <c r="P47">
-        <v>0.76600000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="Q47">
-        <v>0.76400000000000001</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="R47">
-        <v>0.88200000000000001</v>
+        <v>0.60799999999999998</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B48">
-        <v>0.34</v>
+        <v>0.41</v>
       </c>
       <c r="C48">
-        <v>0.45</v>
+        <v>0.49</v>
       </c>
       <c r="D48">
-        <v>0.53</v>
+        <v>0.59</v>
       </c>
       <c r="E48">
         <v>0.63</v>
       </c>
       <c r="F48">
-        <v>0.63</v>
+        <v>0.67</v>
       </c>
       <c r="G48">
-        <v>0.59</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="H48">
-        <v>0.76</v>
+        <v>0.81</v>
       </c>
       <c r="I48">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="K48">
-        <v>0.28799999999999998</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="L48">
-        <v>0.39200000000000002</v>
+        <v>0.442</v>
       </c>
       <c r="M48">
-        <v>0.51800000000000002</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="N48">
-        <v>0.63400000000000001</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="O48">
-        <v>0.68799999999999994</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="P48">
-        <v>0.752</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="Q48">
-        <v>0.74399999999999999</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="R48">
-        <v>0.88600000000000001</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B49">
-        <v>0.36</v>
+        <v>0.33</v>
       </c>
       <c r="C49">
-        <v>0.44</v>
+        <v>0.35</v>
       </c>
       <c r="D49">
-        <v>0.51</v>
+        <v>0.49</v>
       </c>
       <c r="E49">
-        <v>0.63</v>
+        <v>0.39</v>
       </c>
       <c r="F49">
-        <v>0.64</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G49">
-        <v>0.65</v>
+        <v>0.61</v>
       </c>
       <c r="H49">
-        <v>0.75</v>
+        <v>0.61</v>
       </c>
       <c r="I49">
-        <v>0.94</v>
+        <v>0.84</v>
       </c>
       <c r="K49">
-        <v>0.32200000000000001</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="L49">
-        <v>0.39200000000000002</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="M49">
-        <v>0.53</v>
+        <v>0.42799999999999999</v>
       </c>
       <c r="N49">
-        <v>0.63200000000000001</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="O49">
-        <v>0.69399999999999995</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="P49">
-        <v>0.75800000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="Q49">
-        <v>0.76400000000000001</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="R49">
-        <v>0.88</v>
+        <v>0.72799999999999998</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B50">
-        <v>0.24</v>
+        <v>0.35</v>
       </c>
       <c r="C50">
-        <v>0.38</v>
+        <v>0.44</v>
       </c>
       <c r="D50">
-        <v>0.49</v>
+        <v>0.54</v>
       </c>
       <c r="E50">
-        <v>0.43</v>
+        <v>0.63</v>
       </c>
       <c r="F50">
-        <v>0.49</v>
+        <v>0.65</v>
       </c>
       <c r="G50">
-        <v>0.64</v>
+        <v>0.67</v>
       </c>
       <c r="H50">
-        <v>0.52</v>
+        <v>0.77</v>
       </c>
       <c r="I50">
-        <v>0.62</v>
+        <v>0.94</v>
       </c>
       <c r="K50">
-        <v>0.26800000000000002</v>
+        <v>0.316</v>
       </c>
       <c r="L50">
-        <v>0.33400000000000002</v>
+        <v>0.39</v>
       </c>
       <c r="M50">
-        <v>0.44</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="N50">
-        <v>0.46400000000000002</v>
+        <v>0.63</v>
       </c>
       <c r="O50">
-        <v>0.496</v>
+        <v>0.69399999999999995</v>
       </c>
       <c r="P50">
-        <v>0.51800000000000002</v>
+        <v>0.76600000000000001</v>
       </c>
       <c r="Q50">
-        <v>0.53400000000000003</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="R50">
-        <v>0.59</v>
+        <v>0.88200000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51">
+        <v>0.34</v>
+      </c>
+      <c r="C51">
+        <v>0.45</v>
+      </c>
+      <c r="D51">
+        <v>0.53</v>
+      </c>
+      <c r="E51">
+        <v>0.63</v>
+      </c>
+      <c r="F51">
+        <v>0.63</v>
+      </c>
+      <c r="G51">
+        <v>0.59</v>
+      </c>
+      <c r="H51">
+        <v>0.76</v>
+      </c>
+      <c r="I51">
+        <v>0.9</v>
+      </c>
+      <c r="K51">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="L51">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="M51">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="N51">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="O51">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="P51">
+        <v>0.752</v>
+      </c>
+      <c r="Q51">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="R51">
+        <v>0.88600000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52">
+        <v>0.36</v>
+      </c>
+      <c r="C52">
+        <v>0.44</v>
+      </c>
+      <c r="D52">
+        <v>0.51</v>
+      </c>
+      <c r="E52">
+        <v>0.63</v>
+      </c>
+      <c r="F52">
+        <v>0.64</v>
+      </c>
+      <c r="G52">
+        <v>0.65</v>
+      </c>
+      <c r="H52">
+        <v>0.75</v>
+      </c>
+      <c r="I52">
+        <v>0.94</v>
+      </c>
+      <c r="K52">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="L52">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="M52">
+        <v>0.53</v>
+      </c>
+      <c r="N52">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="O52">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="P52">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="Q52">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="R52">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53">
+        <v>0.24</v>
+      </c>
+      <c r="C53">
+        <v>0.38</v>
+      </c>
+      <c r="D53">
+        <v>0.49</v>
+      </c>
+      <c r="E53">
+        <v>0.43</v>
+      </c>
+      <c r="F53">
+        <v>0.49</v>
+      </c>
+      <c r="G53">
+        <v>0.64</v>
+      </c>
+      <c r="H53">
+        <v>0.52</v>
+      </c>
+      <c r="I53">
+        <v>0.62</v>
+      </c>
+      <c r="K53">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="L53">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="M53">
+        <v>0.44</v>
+      </c>
+      <c r="N53">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="O53">
+        <v>0.496</v>
+      </c>
+      <c r="P53">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="Q53">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="R53">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
         <v>29</v>
       </c>
-      <c r="B51">
+      <c r="B54">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C51">
+      <c r="C54">
         <v>0.37</v>
       </c>
-      <c r="D51">
+      <c r="D54">
         <v>0.46</v>
       </c>
-      <c r="E51">
+      <c r="E54">
         <v>0.49</v>
       </c>
-      <c r="F51">
+      <c r="F54">
         <v>0.44</v>
       </c>
-      <c r="G51">
+      <c r="G54">
         <v>0.48</v>
       </c>
-      <c r="H51">
+      <c r="H54">
         <v>0.51</v>
       </c>
-      <c r="I51">
+      <c r="I54">
         <v>0.69</v>
       </c>
-      <c r="K51">
+      <c r="K54">
         <v>0.26400000000000001</v>
       </c>
-      <c r="L51">
+      <c r="L54">
         <v>0.34399999999999997</v>
       </c>
-      <c r="M51">
+      <c r="M54">
         <v>0.42</v>
       </c>
-      <c r="N51">
+      <c r="N54">
         <v>0.48399999999999999</v>
       </c>
-      <c r="O51">
+      <c r="O54">
         <v>0.53800000000000003</v>
       </c>
-      <c r="P51">
+      <c r="P54">
         <v>0.52400000000000002</v>
       </c>
-      <c r="Q51">
+      <c r="Q54">
         <v>0.50600000000000001</v>
       </c>
-      <c r="R51">
+      <c r="R54">
         <v>0.59399999999999997</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B53" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" s="3">
-        <v>3</v>
-      </c>
-      <c r="C54" s="3">
-        <v>4</v>
-      </c>
-      <c r="D54" s="3">
-        <v>5</v>
-      </c>
-      <c r="E54" s="3">
-        <v>6</v>
-      </c>
-      <c r="F54" s="3">
-        <v>7</v>
-      </c>
-      <c r="G54" s="3">
-        <v>8</v>
-      </c>
-      <c r="H54" s="3">
-        <v>9</v>
-      </c>
-      <c r="I54" s="3">
-        <v>10</v>
-      </c>
-      <c r="J54" s="5"/>
-      <c r="K54" s="3">
-        <v>3</v>
-      </c>
-      <c r="L54" s="3">
-        <v>4</v>
-      </c>
-      <c r="M54" s="3">
-        <v>5</v>
-      </c>
-      <c r="N54" s="3">
-        <v>6</v>
-      </c>
-      <c r="O54" s="3">
-        <v>7</v>
-      </c>
-      <c r="P54" s="3">
-        <v>8</v>
-      </c>
-      <c r="Q54" s="3">
-        <v>9</v>
-      </c>
-      <c r="R54" s="3">
-        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>1</v>
-      </c>
-      <c r="B55">
-        <v>0.57666666666666699</v>
-      </c>
-      <c r="C55">
-        <v>0.49249999999999999</v>
+        <v>33</v>
       </c>
       <c r="D55">
-        <v>0.46199999999999902</v>
+        <v>0.61</v>
       </c>
       <c r="E55">
-        <v>0.44666666666666599</v>
+        <v>0.64</v>
       </c>
       <c r="F55">
-        <v>0.41857142857142798</v>
+        <v>0.71</v>
       </c>
       <c r="G55">
-        <v>0.36375000000000002</v>
-      </c>
-      <c r="H55">
-        <v>0.378888888888888</v>
+        <v>0.75</v>
+      </c>
+      <c r="H55" s="5">
+        <v>0.81</v>
       </c>
       <c r="I55">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="K55">
-        <v>0.53866666666666696</v>
-      </c>
-      <c r="L55">
-        <v>0.495</v>
+        <v>0.85</v>
       </c>
       <c r="M55">
-        <v>0.45760000000000001</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="N55">
-        <v>0.44</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="O55">
-        <v>0.40971428571428398</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="P55">
-        <v>0.38750000000000001</v>
+        <v>0.754</v>
       </c>
       <c r="Q55">
-        <v>0.35777777777777903</v>
+        <v>0.754</v>
       </c>
       <c r="R55">
-        <v>0.36059999999999898</v>
+        <v>0.80400000000000005</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56">
-        <v>0.55666666666666698</v>
-      </c>
-      <c r="C56">
-        <v>0.4375</v>
+        <v>34</v>
       </c>
       <c r="D56">
-        <v>0.45199999999999901</v>
+        <v>0.69</v>
       </c>
       <c r="E56">
-        <v>0.396666666666666</v>
+        <v>0.74</v>
       </c>
       <c r="F56">
-        <v>0.38857142857142801</v>
+        <v>0.75</v>
       </c>
       <c r="G56">
-        <v>0.39250000000000002</v>
-      </c>
-      <c r="H56">
-        <v>0.39777777777777701</v>
+        <v>0.92</v>
+      </c>
+      <c r="H56" s="5">
+        <v>1.1000000000000001</v>
       </c>
       <c r="I56">
-        <v>0.43099999999999999</v>
-      </c>
-      <c r="K56">
-        <v>0.51</v>
-      </c>
-      <c r="L56">
-        <v>0.46100000000000002</v>
+        <v>1.06</v>
       </c>
       <c r="M56">
-        <v>0.44440000000000002</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="N56">
-        <v>0.41499999999999998</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="O56">
-        <v>0.40685714285714197</v>
+        <v>0.88800000000000001</v>
       </c>
       <c r="P56">
-        <v>0.38800000000000001</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="Q56">
-        <v>0.36822222222222201</v>
+        <v>1.004</v>
       </c>
       <c r="R56">
-        <v>0.37639999999999901</v>
+        <v>1.026</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A57" t="s">
+      <c r="B57" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="3">
         <v>3</v>
       </c>
-      <c r="B57">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="C57">
-        <v>0.47749999999999998</v>
-      </c>
-      <c r="D57">
-        <v>0.48</v>
-      </c>
-      <c r="E57">
-        <v>0.42166666666666602</v>
-      </c>
-      <c r="F57">
-        <v>0.4</v>
-      </c>
-      <c r="G57">
-        <v>0.37</v>
-      </c>
-      <c r="H57">
-        <v>0.37555555555555498</v>
-      </c>
-      <c r="I57">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="K57">
-        <v>0.53800000000000103</v>
-      </c>
-      <c r="L57">
-        <v>0.47749999999999998</v>
-      </c>
-      <c r="M57">
-        <v>0.44719999999999999</v>
-      </c>
-      <c r="N57">
-        <v>0.42066666666666602</v>
-      </c>
-      <c r="O57">
-        <v>0.39399999999999902</v>
-      </c>
-      <c r="P57">
-        <v>0.371</v>
-      </c>
-      <c r="Q57">
-        <v>0.34822222222222299</v>
-      </c>
-      <c r="R57">
-        <v>0.345799999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A58" t="s">
+      <c r="C58" s="3">
         <v>4</v>
       </c>
-      <c r="B58">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="C58">
-        <v>0.435</v>
-      </c>
-      <c r="D58">
-        <v>0.435999999999999</v>
-      </c>
-      <c r="E58">
-        <v>0.42333333333333301</v>
-      </c>
-      <c r="F58">
-        <v>0.377142857142857</v>
-      </c>
-      <c r="G58">
-        <v>0.3775</v>
-      </c>
-      <c r="H58">
-        <v>0.38999999999999901</v>
-      </c>
-      <c r="I58">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="K58">
-        <v>0.51266666666666705</v>
-      </c>
-      <c r="L58">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="M58">
-        <v>0.44040000000000001</v>
-      </c>
-      <c r="N58">
-        <v>0.41066666666666601</v>
-      </c>
-      <c r="O58">
-        <v>0.39914285714285602</v>
-      </c>
-      <c r="P58">
-        <v>0.38124999999999998</v>
-      </c>
-      <c r="Q58">
-        <v>0.355333333333334</v>
-      </c>
-      <c r="R58">
-        <v>0.36879999999999902</v>
+      <c r="D58" s="3">
+        <v>5</v>
+      </c>
+      <c r="E58" s="3">
+        <v>6</v>
+      </c>
+      <c r="F58" s="3">
+        <v>7</v>
+      </c>
+      <c r="G58" s="3">
+        <v>8</v>
+      </c>
+      <c r="H58" s="3">
+        <v>9</v>
+      </c>
+      <c r="I58" s="3">
+        <v>10</v>
+      </c>
+      <c r="J58" s="5"/>
+      <c r="K58" s="3">
+        <v>3</v>
+      </c>
+      <c r="L58" s="3">
+        <v>4</v>
+      </c>
+      <c r="M58" s="3">
+        <v>5</v>
+      </c>
+      <c r="N58" s="3">
+        <v>6</v>
+      </c>
+      <c r="O58" s="3">
+        <v>7</v>
+      </c>
+      <c r="P58" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q58" s="3">
+        <v>9</v>
+      </c>
+      <c r="R58" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B59">
-        <v>0.53</v>
+        <v>0.57666666666666699</v>
       </c>
       <c r="C59">
-        <v>0.56499999999999995</v>
+        <v>0.49249999999999999</v>
       </c>
       <c r="D59">
-        <v>0.53200000000000003</v>
+        <v>0.46199999999999902</v>
       </c>
       <c r="E59">
-        <v>0.51833333333333298</v>
+        <v>0.44666666666666599</v>
       </c>
       <c r="F59">
-        <v>0.51142857142857101</v>
+        <v>0.41857142857142798</v>
       </c>
       <c r="G59">
-        <v>0.49625000000000002</v>
+        <v>0.36375000000000002</v>
       </c>
       <c r="H59">
-        <v>0.51111111111111096</v>
+        <v>0.378888888888888</v>
       </c>
       <c r="I59">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="K59">
+        <v>0.53866666666666696</v>
+      </c>
+      <c r="L59">
         <v>0.495</v>
       </c>
-      <c r="K59">
-        <v>0.53133333333333399</v>
-      </c>
-      <c r="L59">
-        <v>0.52749999999999997</v>
-      </c>
       <c r="M59">
-        <v>0.5232</v>
+        <v>0.45760000000000001</v>
       </c>
       <c r="N59">
-        <v>0.52333333333333298</v>
+        <v>0.44</v>
       </c>
       <c r="O59">
-        <v>0.51171428571428501</v>
+        <v>0.40971428571428398</v>
       </c>
       <c r="P59">
-        <v>0.499</v>
+        <v>0.38750000000000001</v>
       </c>
       <c r="Q59">
-        <v>0.49866666666666598</v>
+        <v>0.35777777777777903</v>
       </c>
       <c r="R59">
-        <v>0.50139999999999996</v>
+        <v>0.36059999999999898</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B60">
-        <v>0.46333333333333299</v>
+        <v>0.55666666666666698</v>
       </c>
       <c r="C60">
+        <v>0.4375</v>
+      </c>
+      <c r="D60">
+        <v>0.45199999999999901</v>
+      </c>
+      <c r="E60">
+        <v>0.396666666666666</v>
+      </c>
+      <c r="F60">
+        <v>0.38857142857142801</v>
+      </c>
+      <c r="G60">
         <v>0.39250000000000002</v>
       </c>
-      <c r="D60">
-        <v>0.371999999999999</v>
-      </c>
-      <c r="E60">
-        <v>0.37166666666666598</v>
-      </c>
-      <c r="F60">
-        <v>0.28142857142857097</v>
-      </c>
-      <c r="G60">
-        <v>0.33500000000000002</v>
-      </c>
       <c r="H60">
-        <v>0.28888888888888797</v>
+        <v>0.39777777777777701</v>
       </c>
       <c r="I60">
-        <v>0.33200000000000002</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="K60">
-        <v>0.460666666666668</v>
+        <v>0.51</v>
       </c>
       <c r="L60">
-        <v>0.38850000000000001</v>
+        <v>0.46100000000000002</v>
       </c>
       <c r="M60">
-        <v>0.35999999999999899</v>
+        <v>0.44440000000000002</v>
       </c>
       <c r="N60">
-        <v>0.34866666666666601</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="O60">
-        <v>0.32485714285714101</v>
+        <v>0.40685714285714197</v>
       </c>
       <c r="P60">
-        <v>0.30775000000000002</v>
+        <v>0.38800000000000001</v>
       </c>
       <c r="Q60">
-        <v>0.30933333333333402</v>
+        <v>0.36822222222222201</v>
       </c>
       <c r="R60">
-        <v>0.311999999999998</v>
+        <v>0.37639999999999901</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B61">
-        <v>0.49</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="C61">
-        <v>0.38250000000000001</v>
+        <v>0.47749999999999998</v>
       </c>
       <c r="D61">
-        <v>0.35399999999999898</v>
+        <v>0.48</v>
       </c>
       <c r="E61">
-        <v>0.30166666666666597</v>
+        <v>0.42166666666666602</v>
       </c>
       <c r="F61">
-        <v>0.26999999999999902</v>
+        <v>0.4</v>
       </c>
       <c r="G61">
-        <v>0.25624999999999998</v>
+        <v>0.37</v>
       </c>
       <c r="H61">
-        <v>0.24666666666666601</v>
+        <v>0.37555555555555498</v>
       </c>
       <c r="I61">
-        <v>0.253</v>
+        <v>0.40600000000000003</v>
       </c>
       <c r="K61">
-        <v>0.45466666666666899</v>
+        <v>0.53800000000000103</v>
       </c>
       <c r="L61">
-        <v>0.3775</v>
+        <v>0.47749999999999998</v>
       </c>
       <c r="M61">
-        <v>0.3392</v>
+        <v>0.44719999999999999</v>
       </c>
       <c r="N61">
-        <v>0.30733333333333301</v>
+        <v>0.42066666666666602</v>
       </c>
       <c r="O61">
-        <v>0.28457142857142698</v>
+        <v>0.39399999999999902</v>
       </c>
       <c r="P61">
-        <v>0.25974999999999998</v>
+        <v>0.371</v>
       </c>
       <c r="Q61">
-        <v>0.24022222222219999</v>
+        <v>0.34822222222222299</v>
       </c>
       <c r="R61">
-        <v>0.24919999999999901</v>
+        <v>0.345799999999999</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B62">
-        <v>0.44666666666666699</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C62">
-        <v>0.35749999999999998</v>
+        <v>0.435</v>
       </c>
       <c r="D62">
-        <v>0.31999999999999901</v>
+        <v>0.435999999999999</v>
       </c>
       <c r="E62">
-        <v>0.25166666666666598</v>
+        <v>0.42333333333333301</v>
       </c>
       <c r="F62">
-        <v>0.247142857142856</v>
+        <v>0.377142857142857</v>
       </c>
       <c r="G62">
-        <v>0.25874999999999998</v>
+        <v>0.3775</v>
       </c>
       <c r="H62">
-        <v>0.23555555555555499</v>
+        <v>0.38999999999999901</v>
       </c>
       <c r="I62">
-        <v>0.23799999999999999</v>
+        <v>0.41699999999999998</v>
       </c>
       <c r="K62">
-        <v>0.42666666666666803</v>
+        <v>0.51266666666666705</v>
       </c>
       <c r="L62">
-        <v>0.34549999999999997</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="M62">
-        <v>0.30680000000000002</v>
+        <v>0.44040000000000001</v>
       </c>
       <c r="N62">
-        <v>0.28266666666666601</v>
+        <v>0.41066666666666601</v>
       </c>
       <c r="O62">
-        <v>0.26371428571428501</v>
+        <v>0.39914285714285602</v>
       </c>
       <c r="P62">
-        <v>0.23574999999999999</v>
+        <v>0.38124999999999998</v>
       </c>
       <c r="Q62">
-        <v>0.22177777777777799</v>
+        <v>0.355333333333334</v>
       </c>
       <c r="R62">
-        <v>0.226799999999999</v>
+        <v>0.36879999999999902</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B63">
-        <v>0.456666666666667</v>
+        <v>0.53</v>
       </c>
       <c r="C63">
-        <v>0.36249999999999999</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="D63">
-        <v>0.33399999999999902</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="E63">
-        <v>0.293333333333333</v>
+        <v>0.51833333333333298</v>
       </c>
       <c r="F63">
-        <v>0.25714285714285601</v>
+        <v>0.51142857142857101</v>
       </c>
       <c r="G63">
-        <v>0.26124999999999998</v>
+        <v>0.49625000000000002</v>
       </c>
       <c r="H63">
-        <v>0.24777777777777699</v>
+        <v>0.51111111111111096</v>
       </c>
       <c r="I63">
-        <v>0.253</v>
+        <v>0.495</v>
       </c>
       <c r="K63">
-        <v>0.438000000000001</v>
+        <v>0.53133333333333399</v>
       </c>
       <c r="L63">
-        <v>0.35749999999999998</v>
+        <v>0.52749999999999997</v>
       </c>
       <c r="M63">
-        <v>0.32519999999999999</v>
+        <v>0.5232</v>
       </c>
       <c r="N63">
-        <v>0.3</v>
+        <v>0.52333333333333298</v>
       </c>
       <c r="O63">
-        <v>0.28114285714285597</v>
+        <v>0.51171428571428501</v>
       </c>
       <c r="P63">
-        <v>0.25474999999999998</v>
+        <v>0.499</v>
       </c>
       <c r="Q63">
-        <v>0.23488888888889001</v>
+        <v>0.49866666666666598</v>
       </c>
       <c r="R63">
-        <v>0.245199999999999</v>
+        <v>0.50139999999999996</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B64">
-        <v>0.45</v>
+        <v>0.46333333333333299</v>
       </c>
       <c r="C64">
-        <v>0.3725</v>
+        <v>0.39250000000000002</v>
       </c>
       <c r="D64">
-        <v>0.33599999999999902</v>
+        <v>0.371999999999999</v>
       </c>
       <c r="E64">
-        <v>0.293333333333333</v>
+        <v>0.37166666666666598</v>
       </c>
       <c r="F64">
-        <v>0.254285714285714</v>
+        <v>0.28142857142857097</v>
       </c>
       <c r="G64">
-        <v>0.2525</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="H64">
-        <v>0.24222222222222201</v>
+        <v>0.28888888888888797</v>
       </c>
       <c r="I64">
-        <v>0.249</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="K64">
-        <v>0.42866666666666797</v>
+        <v>0.460666666666668</v>
       </c>
       <c r="L64">
-        <v>0.35599999999999998</v>
+        <v>0.38850000000000001</v>
       </c>
       <c r="M64">
-        <v>0.3236</v>
+        <v>0.35999999999999899</v>
       </c>
       <c r="N64">
-        <v>0.29699999999999999</v>
+        <v>0.34866666666666601</v>
       </c>
       <c r="O64">
-        <v>0.27971428571428503</v>
+        <v>0.32485714285714101</v>
       </c>
       <c r="P64">
-        <v>0.25374999999999998</v>
+        <v>0.30775000000000002</v>
       </c>
       <c r="Q64">
-        <v>0.23200000000000101</v>
+        <v>0.30933333333333402</v>
       </c>
       <c r="R64">
-        <v>0.244999999999999</v>
+        <v>0.311999999999998</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B65">
-        <v>0.46</v>
+        <v>0.49</v>
       </c>
       <c r="C65">
-        <v>0.36249999999999999</v>
+        <v>0.38250000000000001</v>
       </c>
       <c r="D65">
-        <v>0.32799999999999901</v>
+        <v>0.35399999999999898</v>
       </c>
       <c r="E65">
-        <v>0.30666666666666598</v>
+        <v>0.30166666666666597</v>
       </c>
       <c r="F65">
-        <v>0.26428571428571401</v>
+        <v>0.26999999999999902</v>
       </c>
       <c r="G65">
-        <v>0.26374999999999998</v>
+        <v>0.25624999999999998</v>
       </c>
       <c r="H65">
-        <v>0.24444444444444399</v>
+        <v>0.24666666666666601</v>
       </c>
       <c r="I65">
-        <v>0.26400000000000001</v>
+        <v>0.253</v>
       </c>
       <c r="K65">
-        <v>0.440000000000001</v>
+        <v>0.45466666666666899</v>
       </c>
       <c r="L65">
-        <v>0.36049999999999999</v>
+        <v>0.3775</v>
       </c>
       <c r="M65">
-        <v>0.32799999999999901</v>
+        <v>0.3392</v>
       </c>
       <c r="N65">
-        <v>0.30099999999999999</v>
+        <v>0.30733333333333301</v>
       </c>
       <c r="O65">
-        <v>0.28257142857142797</v>
+        <v>0.28457142857142698</v>
       </c>
       <c r="P65">
-        <v>0.25324999999999998</v>
+        <v>0.25974999999999998</v>
       </c>
       <c r="Q65">
-        <v>0.23733333333333401</v>
+        <v>0.24022222222219999</v>
       </c>
       <c r="R65">
-        <v>0.25059999999999899</v>
+        <v>0.24919999999999901</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B66">
-        <v>0.46</v>
+        <v>0.44666666666666699</v>
       </c>
       <c r="C66">
-        <v>0.39250000000000002</v>
+        <v>0.35749999999999998</v>
       </c>
       <c r="D66">
-        <v>0.371999999999999</v>
+        <v>0.31999999999999901</v>
       </c>
       <c r="E66">
-        <v>0.37166666666666598</v>
+        <v>0.25166666666666598</v>
       </c>
       <c r="F66">
-        <v>0.27999999999999903</v>
+        <v>0.247142857142856</v>
       </c>
       <c r="G66">
-        <v>0.33500000000000002</v>
+        <v>0.25874999999999998</v>
       </c>
       <c r="H66">
-        <v>0.28888888888888797</v>
+        <v>0.23555555555555499</v>
       </c>
       <c r="I66">
-        <v>0.32900000000000001</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="K66">
-        <v>0.45933333333333398</v>
+        <v>0.42666666666666803</v>
       </c>
       <c r="L66">
-        <v>0.38700000000000001</v>
+        <v>0.34549999999999997</v>
       </c>
       <c r="M66">
-        <v>0.360399999999999</v>
+        <v>0.30680000000000002</v>
       </c>
       <c r="N66">
-        <v>0.34766666666666601</v>
+        <v>0.28266666666666601</v>
       </c>
       <c r="O66">
-        <v>0.32399999999999801</v>
+        <v>0.26371428571428501</v>
       </c>
       <c r="P66">
-        <v>0.30625000000000002</v>
+        <v>0.23574999999999999</v>
       </c>
       <c r="Q66">
-        <v>0.30955555555555597</v>
+        <v>0.22177777777777799</v>
       </c>
       <c r="R66">
-        <v>0.31059999999999799</v>
+        <v>0.226799999999999</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67">
+        <v>0.456666666666667</v>
+      </c>
+      <c r="C67">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="D67">
+        <v>0.33399999999999902</v>
+      </c>
+      <c r="E67">
+        <v>0.293333333333333</v>
+      </c>
+      <c r="F67">
+        <v>0.25714285714285601</v>
+      </c>
+      <c r="G67">
+        <v>0.26124999999999998</v>
+      </c>
+      <c r="H67">
+        <v>0.24777777777777699</v>
+      </c>
+      <c r="I67">
+        <v>0.253</v>
+      </c>
+      <c r="K67">
+        <v>0.438000000000001</v>
+      </c>
+      <c r="L67">
+        <v>0.35749999999999998</v>
+      </c>
+      <c r="M67">
+        <v>0.32519999999999999</v>
+      </c>
+      <c r="N67">
+        <v>0.3</v>
+      </c>
+      <c r="O67">
+        <v>0.28114285714285597</v>
+      </c>
+      <c r="P67">
+        <v>0.25474999999999998</v>
+      </c>
+      <c r="Q67">
+        <v>0.23488888888889001</v>
+      </c>
+      <c r="R67">
+        <v>0.245199999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68">
+        <v>0.45</v>
+      </c>
+      <c r="C68">
+        <v>0.3725</v>
+      </c>
+      <c r="D68">
+        <v>0.33599999999999902</v>
+      </c>
+      <c r="E68">
+        <v>0.293333333333333</v>
+      </c>
+      <c r="F68">
+        <v>0.254285714285714</v>
+      </c>
+      <c r="G68">
+        <v>0.2525</v>
+      </c>
+      <c r="H68">
+        <v>0.24222222222222201</v>
+      </c>
+      <c r="I68">
+        <v>0.249</v>
+      </c>
+      <c r="K68">
+        <v>0.42866666666666797</v>
+      </c>
+      <c r="L68">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="M68">
+        <v>0.3236</v>
+      </c>
+      <c r="N68">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="O68">
+        <v>0.27971428571428503</v>
+      </c>
+      <c r="P68">
+        <v>0.25374999999999998</v>
+      </c>
+      <c r="Q68">
+        <v>0.23200000000000101</v>
+      </c>
+      <c r="R68">
+        <v>0.244999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69">
+        <v>0.46</v>
+      </c>
+      <c r="C69">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="D69">
+        <v>0.32799999999999901</v>
+      </c>
+      <c r="E69">
+        <v>0.30666666666666598</v>
+      </c>
+      <c r="F69">
+        <v>0.26428571428571401</v>
+      </c>
+      <c r="G69">
+        <v>0.26374999999999998</v>
+      </c>
+      <c r="H69">
+        <v>0.24444444444444399</v>
+      </c>
+      <c r="I69">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="K69">
+        <v>0.440000000000001</v>
+      </c>
+      <c r="L69">
+        <v>0.36049999999999999</v>
+      </c>
+      <c r="M69">
+        <v>0.32799999999999901</v>
+      </c>
+      <c r="N69">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="O69">
+        <v>0.28257142857142797</v>
+      </c>
+      <c r="P69">
+        <v>0.25324999999999998</v>
+      </c>
+      <c r="Q69">
+        <v>0.23733333333333401</v>
+      </c>
+      <c r="R69">
+        <v>0.25059999999999899</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70">
+        <v>0.46</v>
+      </c>
+      <c r="C70">
+        <v>0.39250000000000002</v>
+      </c>
+      <c r="D70">
+        <v>0.371999999999999</v>
+      </c>
+      <c r="E70">
+        <v>0.37166666666666598</v>
+      </c>
+      <c r="F70">
+        <v>0.27999999999999903</v>
+      </c>
+      <c r="G70">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H70">
+        <v>0.28888888888888797</v>
+      </c>
+      <c r="I70">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="K70">
+        <v>0.45933333333333398</v>
+      </c>
+      <c r="L70">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="M70">
+        <v>0.360399999999999</v>
+      </c>
+      <c r="N70">
+        <v>0.34766666666666601</v>
+      </c>
+      <c r="O70">
+        <v>0.32399999999999801</v>
+      </c>
+      <c r="P70">
+        <v>0.30625000000000002</v>
+      </c>
+      <c r="Q70">
+        <v>0.30955555555555597</v>
+      </c>
+      <c r="R70">
+        <v>0.31059999999999799</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
         <v>29</v>
       </c>
-      <c r="B67">
+      <c r="B71">
         <v>0.43</v>
       </c>
-      <c r="C67">
+      <c r="C71">
         <v>0.35749999999999998</v>
       </c>
-      <c r="D67">
+      <c r="D71">
         <v>0.309999999999999</v>
       </c>
-      <c r="E67">
+      <c r="E71">
         <v>0.24833333333333299</v>
       </c>
-      <c r="F67">
+      <c r="F71">
         <v>0.221428571428571</v>
       </c>
-      <c r="G67">
+      <c r="G71">
         <v>0.21</v>
       </c>
-      <c r="H67">
+      <c r="H71">
         <v>0.18222222222222101</v>
       </c>
-      <c r="I67">
+      <c r="I71">
         <v>0.188999999999999</v>
       </c>
-      <c r="K67">
+      <c r="K71">
         <v>0.421333333333335</v>
       </c>
-      <c r="L67">
+      <c r="L71">
         <v>0.34300000000000003</v>
       </c>
-      <c r="M67">
+      <c r="M71">
         <v>0.29599999999999999</v>
       </c>
-      <c r="N67">
+      <c r="N71">
         <v>0.26066666666666699</v>
       </c>
-      <c r="O67">
+      <c r="O71">
         <v>0.23257142857142801</v>
       </c>
-      <c r="P67">
+      <c r="P71">
         <v>0.20324999999999999</v>
       </c>
-      <c r="Q67">
+      <c r="Q71">
         <v>0.183555555555557</v>
       </c>
-      <c r="R67">
+      <c r="R71">
         <v>0.18039999999999901</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72">
+        <v>0.434</v>
+      </c>
+      <c r="E72">
+        <v>0.40670000000000001</v>
+      </c>
+      <c r="F72">
+        <v>0.44</v>
+      </c>
+      <c r="G72" s="5">
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="H72">
+        <v>0.37330000000000002</v>
+      </c>
+      <c r="I72">
+        <v>0.316</v>
+      </c>
+      <c r="M72">
+        <v>0.4264</v>
+      </c>
+      <c r="N72">
+        <v>0.40529999999999999</v>
+      </c>
+      <c r="O72">
+        <v>0.39140000000000003</v>
+      </c>
+      <c r="P72">
+        <v>0.37130000000000002</v>
+      </c>
+      <c r="Q72">
+        <v>0.34329999999999999</v>
+      </c>
+      <c r="R72">
+        <v>0.31419999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="E73">
+        <v>0.43330000000000002</v>
+      </c>
+      <c r="F73">
+        <v>0.37290000000000001</v>
+      </c>
+      <c r="G73" s="5">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="H73">
+        <v>0.38109999999999999</v>
+      </c>
+      <c r="I73">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="M73">
+        <v>0.44640000000000002</v>
+      </c>
+      <c r="N73">
+        <v>0.40670000000000001</v>
+      </c>
+      <c r="O73">
+        <v>0.40510000000000002</v>
+      </c>
+      <c r="P73">
+        <v>0.38869999999999999</v>
+      </c>
+      <c r="Q73">
+        <v>0.3589</v>
+      </c>
+      <c r="R73">
+        <v>0.33760000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -7916,8 +8252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:I47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D45" activeCellId="1" sqref="D40:I42 D45:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7942,7 +8278,7 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -8234,7 +8570,7 @@
       </c>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -8526,7 +8862,7 @@
       </c>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -8818,7 +9154,7 @@
       </c>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -9936,15 +10272,365 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:H8"/>
+      <selection activeCell="F13" sqref="F13:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="4:16" x14ac:dyDescent="0.15">
+      <c r="D1">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="E1">
+        <v>0.23150000000000001</v>
+      </c>
+      <c r="F1">
+        <v>0.23350000000000001</v>
+      </c>
+      <c r="G1">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="H1">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="I1">
+        <v>0.19450000000000001</v>
+      </c>
+      <c r="K1">
+        <v>0.39861657020719299</v>
+      </c>
+      <c r="L1">
+        <v>0.40328575620586299</v>
+      </c>
+      <c r="M1">
+        <v>0.38580773804299801</v>
+      </c>
+      <c r="N1">
+        <v>0.40925078504212298</v>
+      </c>
+      <c r="O1">
+        <v>0.406263404457128</v>
+      </c>
+      <c r="P1">
+        <v>0.40371221339950802</v>
+      </c>
+    </row>
+    <row r="2" spans="4:16" x14ac:dyDescent="0.15">
+      <c r="D2">
+        <v>0.1305</v>
+      </c>
+      <c r="E2">
+        <v>0.114</v>
+      </c>
+      <c r="F2">
+        <v>0.1055</v>
+      </c>
+      <c r="G2">
+        <v>8.8499999999999995E-2</v>
+      </c>
+      <c r="H2">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="I2">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="K2">
+        <v>0.429067749143618</v>
+      </c>
+      <c r="L2">
+        <v>0.43898890650633698</v>
+      </c>
+      <c r="M2">
+        <v>0.42921890886303299</v>
+      </c>
+      <c r="N2">
+        <v>0.44212848792488402</v>
+      </c>
+      <c r="O2">
+        <v>0.453498176597878</v>
+      </c>
+      <c r="P2">
+        <v>0.44796774421328001</v>
+      </c>
+    </row>
+    <row r="3" spans="4:16" x14ac:dyDescent="0.15">
+      <c r="D3">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.1915</v>
+      </c>
+      <c r="F3">
+        <v>0.17949999999999999</v>
+      </c>
+      <c r="G3">
+        <v>0.1515</v>
+      </c>
+      <c r="H3">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="I3">
+        <v>0.13250000000000001</v>
+      </c>
+      <c r="K3">
+        <v>0.39479619055867798</v>
+      </c>
+      <c r="L3">
+        <v>0.399104236909259</v>
+      </c>
+      <c r="M3">
+        <v>0.39237173480754001</v>
+      </c>
+      <c r="N3">
+        <v>0.40525185665058699</v>
+      </c>
+      <c r="O3">
+        <v>0.41596335936927697</v>
+      </c>
+      <c r="P3">
+        <v>0.40176966737457098</v>
+      </c>
+    </row>
+    <row r="4" spans="4:16" x14ac:dyDescent="0.15">
+      <c r="D4">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="E4">
+        <v>0.27</v>
+      </c>
+      <c r="F4">
+        <v>0.26450000000000001</v>
+      </c>
+      <c r="G4">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="H4">
+        <v>0.24049999999999999</v>
+      </c>
+      <c r="I4">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="K4">
+        <v>0.36217114860340499</v>
+      </c>
+      <c r="L4">
+        <v>0.39326456804665</v>
+      </c>
+      <c r="M4">
+        <v>0.38553562174661199</v>
+      </c>
+      <c r="N4">
+        <v>0.37684997900099299</v>
+      </c>
+      <c r="O4">
+        <v>0.39810674741914198</v>
+      </c>
+      <c r="P4">
+        <v>0.41030379770861802</v>
+      </c>
+    </row>
+    <row r="5" spans="4:16" x14ac:dyDescent="0.15">
+      <c r="D5">
+        <v>0.24</v>
+      </c>
+      <c r="E5">
+        <v>0.19550000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.184</v>
+      </c>
+      <c r="G5">
+        <v>0.1905</v>
+      </c>
+      <c r="H5">
+        <v>0.1855</v>
+      </c>
+      <c r="I5">
+        <v>0.15</v>
+      </c>
+      <c r="K5">
+        <v>0.443243014747286</v>
+      </c>
+      <c r="L5">
+        <v>0.46244460545866001</v>
+      </c>
+      <c r="M5">
+        <v>0.45748063645069798</v>
+      </c>
+      <c r="N5">
+        <v>0.45229388362057199</v>
+      </c>
+      <c r="O5">
+        <v>0.46873161652335699</v>
+      </c>
+      <c r="P5">
+        <v>0.48714165704030199</v>
+      </c>
+    </row>
+    <row r="6" spans="4:16" x14ac:dyDescent="0.15">
+      <c r="D6">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.19750000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.186</v>
+      </c>
+      <c r="G6">
+        <v>0.19</v>
+      </c>
+      <c r="H6">
+        <v>0.1835</v>
+      </c>
+      <c r="I6">
+        <v>0.152</v>
+      </c>
+      <c r="K6">
+        <v>0.442764189009556</v>
+      </c>
+      <c r="L6">
+        <v>0.46859032183413601</v>
+      </c>
+      <c r="M6">
+        <v>0.46659979803546398</v>
+      </c>
+      <c r="N6">
+        <v>0.45926038264405</v>
+      </c>
+      <c r="O6">
+        <v>0.478125604352856</v>
+      </c>
+      <c r="P6">
+        <v>0.49647292208846799</v>
+      </c>
+    </row>
+    <row r="13" spans="4:16" x14ac:dyDescent="0.15">
+      <c r="F13">
+        <v>0.33645000000000003</v>
+      </c>
+      <c r="G13">
+        <v>0.33494000000000002</v>
+      </c>
+      <c r="H13">
+        <v>0.29873333333333502</v>
+      </c>
+      <c r="I13">
+        <v>0.30708571428571502</v>
+      </c>
+      <c r="J13">
+        <v>0.30137499999999701</v>
+      </c>
+      <c r="K13">
+        <v>0.29202222222222302</v>
+      </c>
+    </row>
+    <row r="14" spans="4:16" x14ac:dyDescent="0.15">
+      <c r="F14">
+        <v>0.48809999999999798</v>
+      </c>
+      <c r="G14">
+        <v>0.47109999999999802</v>
+      </c>
+      <c r="H14">
+        <v>0.46543333333333298</v>
+      </c>
+      <c r="I14">
+        <v>0.46678571428571403</v>
+      </c>
+      <c r="J14">
+        <v>0.48216249999999899</v>
+      </c>
+      <c r="K14">
+        <v>0.47457777777777899</v>
+      </c>
+    </row>
+    <row r="15" spans="4:16" x14ac:dyDescent="0.15">
+      <c r="F15">
+        <v>0.406249999999997</v>
+      </c>
+      <c r="G15">
+        <v>0.38819999999999999</v>
+      </c>
+      <c r="H15">
+        <v>0.380516666666667</v>
+      </c>
+      <c r="I15">
+        <v>0.37467142857142999</v>
+      </c>
+      <c r="J15">
+        <v>0.38452499999999801</v>
+      </c>
+      <c r="K15">
+        <v>0.37141111111111302</v>
+      </c>
+    </row>
+    <row r="16" spans="4:16" x14ac:dyDescent="0.15">
+      <c r="F16">
+        <v>0.188525000000002</v>
+      </c>
+      <c r="G16">
+        <v>0.193580000000001</v>
+      </c>
+      <c r="H16">
+        <v>0.176933333333334</v>
+      </c>
+      <c r="I16">
+        <v>0.18197142857142901</v>
+      </c>
+      <c r="J16">
+        <v>0.16919999999999899</v>
+      </c>
+      <c r="K16">
+        <v>0.17211111111111099</v>
+      </c>
+    </row>
+    <row r="17" spans="6:11" x14ac:dyDescent="0.15">
+      <c r="F17">
+        <v>0.22137500000000099</v>
+      </c>
+      <c r="G17">
+        <v>0.222000000000001</v>
+      </c>
+      <c r="H17">
+        <v>0.20578333333333401</v>
+      </c>
+      <c r="I17">
+        <v>0.205828571428572</v>
+      </c>
+      <c r="J17">
+        <v>0.192549999999999</v>
+      </c>
+      <c r="K17">
+        <v>0.19731111111111099</v>
+      </c>
+    </row>
+    <row r="18" spans="6:11" x14ac:dyDescent="0.15">
+      <c r="F18">
+        <v>0.21655000000000099</v>
+      </c>
+      <c r="G18">
+        <v>0.21910000000000099</v>
+      </c>
+      <c r="H18">
+        <v>0.20456666666666701</v>
+      </c>
+      <c r="I18">
+        <v>0.20480000000000001</v>
+      </c>
+      <c r="J18">
+        <v>0.19122499999999901</v>
+      </c>
+      <c r="K18">
+        <v>0.196211111111111</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>